<commit_message>
Published state of ETDataset on 8 June 2016
</commit_message>
<xml_diff>
--- a/carriers_source_analyses/wood_pellets.carrier.xlsx
+++ b/carriers_source_analyses/wood_pellets.carrier.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="762" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="23460" tabRatio="762" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="14" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="169">
   <si>
     <t>Source</t>
   </si>
@@ -353,15 +353,9 @@
     <t>residential wood pellets price</t>
   </si>
   <si>
-    <t>17,5 GJ per tonne with tonne costing 135</t>
-  </si>
-  <si>
     <t>Industrial</t>
   </si>
   <si>
-    <t>17,5 GJ per tonne with tonne costing 220</t>
-  </si>
-  <si>
     <t>Residential</t>
   </si>
   <si>
@@ -447,9 +441,6 @@
   </si>
   <si>
     <t>144-145</t>
-  </si>
-  <si>
-    <t>a tonne of woodpellets has 17,5 GJ</t>
   </si>
   <si>
     <t>kg CO2e per tonne woodpellets</t>
@@ -559,6 +550,18 @@
   </si>
   <si>
     <t>start_value</t>
+  </si>
+  <si>
+    <t>a tonne of woodpellets has 17,6 GJ</t>
+  </si>
+  <si>
+    <t>17,6 GJ per tonne with tonne costing 135</t>
+  </si>
+  <si>
+    <t>17,6 GJ per tonne with tonne costing 220</t>
+  </si>
+  <si>
+    <t>Sikkema</t>
   </si>
 </sst>
 </file>
@@ -1734,7 +1737,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="223">
+  <cellXfs count="224">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -2042,6 +2045,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="3" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3283,7 +3287,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="11668952" y="36867612"/>
+          <a:off x="11707052" y="36867612"/>
           <a:ext cx="7355648" cy="8391186"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3792,10 +3796,10 @@
     <row r="4" spans="1:4">
       <c r="A4" s="7"/>
       <c r="B4" s="8" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -3992,28 +3996,28 @@
       <c r="G1" s="35"/>
     </row>
     <row r="2" spans="2:11" ht="15" customHeight="1">
-      <c r="B2" s="211" t="s">
-        <v>162</v>
-      </c>
-      <c r="C2" s="212"/>
-      <c r="D2" s="212"/>
-      <c r="E2" s="213"/>
+      <c r="B2" s="212" t="s">
+        <v>159</v>
+      </c>
+      <c r="C2" s="213"/>
+      <c r="D2" s="213"/>
+      <c r="E2" s="214"/>
       <c r="F2" s="35"/>
       <c r="G2" s="35"/>
     </row>
     <row r="3" spans="2:11">
-      <c r="B3" s="214"/>
-      <c r="C3" s="215"/>
-      <c r="D3" s="215"/>
-      <c r="E3" s="216"/>
+      <c r="B3" s="215"/>
+      <c r="C3" s="216"/>
+      <c r="D3" s="216"/>
+      <c r="E3" s="217"/>
       <c r="F3" s="35"/>
       <c r="G3" s="35"/>
     </row>
     <row r="4" spans="2:11">
-      <c r="B4" s="217"/>
-      <c r="C4" s="218"/>
-      <c r="D4" s="218"/>
-      <c r="E4" s="219"/>
+      <c r="B4" s="218"/>
+      <c r="C4" s="219"/>
+      <c r="D4" s="219"/>
+      <c r="E4" s="220"/>
       <c r="F4" s="35"/>
       <c r="G4" s="35"/>
     </row>
@@ -4066,7 +4070,7 @@
     <row r="9" spans="2:11" s="44" customFormat="1" ht="19" thickBot="1">
       <c r="B9" s="25"/>
       <c r="C9" s="20" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D9" s="33"/>
       <c r="E9" s="20"/>
@@ -4108,33 +4112,33 @@
       </c>
       <c r="E11" s="208">
         <f>'Research data'!G7</f>
-        <v>7.6845303867403318E-3</v>
+        <v>7.7272222222222221E-3</v>
       </c>
       <c r="F11" s="36"/>
       <c r="G11" s="114"/>
       <c r="H11" s="32"/>
       <c r="I11" s="198" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="J11" s="45"/>
     </row>
     <row r="12" spans="2:11" s="44" customFormat="1" ht="19" thickBot="1">
       <c r="B12" s="25"/>
       <c r="C12" s="114" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D12" s="24" t="s">
         <v>53</v>
       </c>
       <c r="E12" s="47">
         <f>'Research data'!G8</f>
-        <v>18.100000000000001</v>
+        <v>18</v>
       </c>
       <c r="F12" s="36"/>
       <c r="G12" s="114"/>
       <c r="H12" s="32"/>
       <c r="I12" s="198" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="J12" s="45"/>
     </row>
@@ -4291,28 +4295,28 @@
       <c r="G1" s="35"/>
     </row>
     <row r="2" spans="2:10" ht="15" customHeight="1">
-      <c r="B2" s="211" t="s">
-        <v>163</v>
-      </c>
-      <c r="C2" s="212"/>
-      <c r="D2" s="212"/>
-      <c r="E2" s="213"/>
+      <c r="B2" s="212" t="s">
+        <v>160</v>
+      </c>
+      <c r="C2" s="213"/>
+      <c r="D2" s="213"/>
+      <c r="E2" s="214"/>
       <c r="F2" s="35"/>
       <c r="G2" s="35"/>
     </row>
     <row r="3" spans="2:10">
-      <c r="B3" s="214"/>
-      <c r="C3" s="215"/>
-      <c r="D3" s="215"/>
-      <c r="E3" s="216"/>
+      <c r="B3" s="215"/>
+      <c r="C3" s="216"/>
+      <c r="D3" s="216"/>
+      <c r="E3" s="217"/>
       <c r="F3" s="35"/>
       <c r="G3" s="35"/>
     </row>
     <row r="4" spans="2:10">
-      <c r="B4" s="220"/>
-      <c r="C4" s="221"/>
-      <c r="D4" s="221"/>
-      <c r="E4" s="222"/>
+      <c r="B4" s="221"/>
+      <c r="C4" s="222"/>
+      <c r="D4" s="222"/>
+      <c r="E4" s="223"/>
       <c r="F4" s="35"/>
       <c r="G4" s="35"/>
     </row>
@@ -4389,7 +4393,7 @@
     <row r="11" spans="2:10" ht="16" thickBot="1">
       <c r="B11" s="40"/>
       <c r="C11" s="209" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D11" s="114"/>
       <c r="E11" s="114"/>
@@ -4534,7 +4538,7 @@
     <row r="18" spans="2:10" ht="16" thickBot="1">
       <c r="B18" s="40"/>
       <c r="C18" s="210" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D18" s="24" t="s">
         <v>1</v>
@@ -4581,10 +4585,10 @@
   <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0">
     <tabColor theme="6" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="B1:S18"/>
+  <dimension ref="B1:U18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4605,14 +4609,16 @@
     <col min="14" max="14" width="2.75" style="66" customWidth="1"/>
     <col min="15" max="15" width="8.5" style="66" customWidth="1"/>
     <col min="16" max="16" width="2.75" style="66" customWidth="1"/>
-    <col min="17" max="17" width="9.625" style="66" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.5" style="66" customWidth="1"/>
     <col min="18" max="18" width="2.75" style="66" customWidth="1"/>
-    <col min="19" max="19" width="60" style="65" customWidth="1"/>
-    <col min="20" max="16384" width="10.625" style="65"/>
+    <col min="19" max="19" width="9.625" style="66" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="2.75" style="66" customWidth="1"/>
+    <col min="21" max="21" width="60" style="65" customWidth="1"/>
+    <col min="22" max="16384" width="10.625" style="65"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19" ht="16" thickBot="1"/>
-    <row r="2" spans="2:19">
+    <row r="1" spans="2:21" ht="16" thickBot="1"/>
+    <row r="2" spans="2:21">
       <c r="B2" s="67"/>
       <c r="C2" s="68"/>
       <c r="D2" s="68"/>
@@ -4630,9 +4636,11 @@
       <c r="P2" s="69"/>
       <c r="Q2" s="69"/>
       <c r="R2" s="69"/>
-      <c r="S2" s="70"/>
-    </row>
-    <row r="3" spans="2:19" s="26" customFormat="1">
+      <c r="S2" s="69"/>
+      <c r="T2" s="69"/>
+      <c r="U2" s="70"/>
+    </row>
+    <row r="3" spans="2:21" s="26" customFormat="1">
       <c r="B3" s="25"/>
       <c r="C3" s="106" t="s">
         <v>30</v>
@@ -4647,7 +4655,7 @@
       </c>
       <c r="H3" s="106"/>
       <c r="I3" s="64" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="J3" s="64"/>
       <c r="K3" s="64" t="s">
@@ -4655,22 +4663,26 @@
       </c>
       <c r="L3" s="64"/>
       <c r="M3" s="64" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="N3" s="64"/>
       <c r="O3" s="64" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="P3" s="64"/>
       <c r="Q3" s="64" t="s">
-        <v>152</v>
+        <v>168</v>
       </c>
       <c r="R3" s="64"/>
-      <c r="S3" s="1" t="s">
+      <c r="S3" s="64" t="s">
+        <v>149</v>
+      </c>
+      <c r="T3" s="64"/>
+      <c r="U3" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="2:19">
+    <row r="4" spans="2:21">
       <c r="B4" s="71"/>
       <c r="C4" s="72"/>
       <c r="D4" s="72"/>
@@ -4688,9 +4700,11 @@
       <c r="P4" s="105"/>
       <c r="Q4" s="103"/>
       <c r="R4" s="105"/>
-      <c r="S4" s="2"/>
-    </row>
-    <row r="5" spans="2:19" ht="16" thickBot="1">
+      <c r="S4" s="103"/>
+      <c r="T4" s="105"/>
+      <c r="U4" s="2"/>
+    </row>
+    <row r="5" spans="2:21" ht="16" thickBot="1">
       <c r="B5" s="71"/>
       <c r="C5" s="20" t="s">
         <v>55</v>
@@ -4710,9 +4724,11 @@
       <c r="P5" s="16"/>
       <c r="Q5" s="16"/>
       <c r="R5" s="16"/>
-      <c r="S5" s="3"/>
-    </row>
-    <row r="6" spans="2:19" ht="16" thickBot="1">
+      <c r="S5" s="16"/>
+      <c r="T5" s="16"/>
+      <c r="U5" s="3"/>
+    </row>
+    <row r="6" spans="2:21" ht="16" thickBot="1">
       <c r="B6" s="71"/>
       <c r="C6" s="118" t="s">
         <v>38</v>
@@ -4740,9 +4756,11 @@
       <c r="P6" s="16"/>
       <c r="Q6" s="16"/>
       <c r="R6" s="16"/>
-      <c r="S6" s="3"/>
-    </row>
-    <row r="7" spans="2:19" s="6" customFormat="1" ht="16" thickBot="1">
+      <c r="S6" s="16"/>
+      <c r="T6" s="16"/>
+      <c r="U6" s="3"/>
+    </row>
+    <row r="7" spans="2:21" s="6" customFormat="1" ht="16" thickBot="1">
       <c r="B7" s="5"/>
       <c r="C7" s="119" t="s">
         <v>39</v>
@@ -4757,8 +4775,8 @@
         <v>54</v>
       </c>
       <c r="G7" s="137">
-        <f>Q7</f>
-        <v>7.6845303867403318E-3</v>
+        <f>S7</f>
+        <v>7.7272222222222221E-3</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="18"/>
@@ -4769,19 +4787,21 @@
       <c r="N7" s="18"/>
       <c r="O7" s="16"/>
       <c r="P7" s="16"/>
-      <c r="Q7" s="207">
+      <c r="Q7" s="16"/>
+      <c r="R7" s="16"/>
+      <c r="S7" s="207">
         <f>Notes!F383</f>
-        <v>7.6845303867403318E-3</v>
-      </c>
-      <c r="R7" s="16"/>
-      <c r="S7" s="186" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="8" spans="2:19" s="6" customFormat="1" ht="16" thickBot="1">
+        <v>7.7272222222222221E-3</v>
+      </c>
+      <c r="T7" s="16"/>
+      <c r="U7" s="186" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21" s="6" customFormat="1" ht="16" thickBot="1">
       <c r="B8" s="5"/>
       <c r="C8" s="119" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D8" s="119" t="s">
         <v>52</v>
@@ -4793,8 +4813,8 @@
         <v>53</v>
       </c>
       <c r="G8" s="46">
-        <f>ROUND(AVERAGE(I8,K8,M8),1)</f>
-        <v>18.100000000000001</v>
+        <f>ROUND(AVERAGE(I8,K8,M8,Q8),1)</f>
+        <v>18</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="47">
@@ -4814,11 +4834,16 @@
       <c r="N8" s="18"/>
       <c r="O8" s="16"/>
       <c r="P8" s="16"/>
-      <c r="Q8" s="16"/>
+      <c r="Q8" s="47">
+        <f>Notes!G189</f>
+        <v>17.600000000000001</v>
+      </c>
       <c r="R8" s="16"/>
-      <c r="S8" s="3"/>
-    </row>
-    <row r="9" spans="2:19" s="6" customFormat="1" ht="16" thickBot="1">
+      <c r="S8" s="16"/>
+      <c r="T8" s="16"/>
+      <c r="U8" s="3"/>
+    </row>
+    <row r="9" spans="2:21" s="6" customFormat="1" ht="16" thickBot="1">
       <c r="B9" s="5"/>
       <c r="C9" s="120" t="s">
         <v>40</v>
@@ -4850,9 +4875,11 @@
       <c r="P9" s="16"/>
       <c r="Q9" s="16"/>
       <c r="R9" s="16"/>
-      <c r="S9" s="3"/>
-    </row>
-    <row r="10" spans="2:19" ht="16" thickBot="1">
+      <c r="S9" s="16"/>
+      <c r="T9" s="16"/>
+      <c r="U9" s="3"/>
+    </row>
+    <row r="10" spans="2:21" ht="16" thickBot="1">
       <c r="B10" s="71"/>
       <c r="C10" s="120" t="s">
         <v>41</v>
@@ -4888,12 +4915,14 @@
         <v>18879000</v>
       </c>
       <c r="P10" s="16"/>
+      <c r="Q10" s="211"/>
       <c r="R10" s="16"/>
-      <c r="S10" s="186" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="11" spans="2:19">
+      <c r="T10" s="16"/>
+      <c r="U10" s="186" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="2:21">
       <c r="B11" s="71"/>
       <c r="C11" s="34"/>
       <c r="D11" s="34"/>
@@ -4911,9 +4940,11 @@
       <c r="P11" s="16"/>
       <c r="Q11" s="16"/>
       <c r="R11" s="16"/>
-      <c r="S11" s="126"/>
-    </row>
-    <row r="12" spans="2:19" ht="16" thickBot="1">
+      <c r="S11" s="16"/>
+      <c r="T11" s="16"/>
+      <c r="U11" s="126"/>
+    </row>
+    <row r="12" spans="2:21" ht="16" thickBot="1">
       <c r="B12" s="71"/>
       <c r="C12" s="20" t="s">
         <v>37</v>
@@ -4933,9 +4964,11 @@
       <c r="P12" s="16"/>
       <c r="Q12" s="16"/>
       <c r="R12" s="16"/>
-      <c r="S12" s="126"/>
-    </row>
-    <row r="13" spans="2:19" ht="16" thickBot="1">
+      <c r="S12" s="16"/>
+      <c r="T12" s="16"/>
+      <c r="U12" s="126"/>
+    </row>
+    <row r="13" spans="2:21" ht="16" thickBot="1">
       <c r="B13" s="71"/>
       <c r="C13" s="121" t="s">
         <v>44</v>
@@ -4963,11 +4996,13 @@
       <c r="P13" s="75"/>
       <c r="Q13" s="18"/>
       <c r="R13" s="75"/>
-      <c r="S13" s="136" t="s">
+      <c r="S13" s="18"/>
+      <c r="T13" s="75"/>
+      <c r="U13" s="136" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="2:19" ht="16" thickBot="1">
+    <row r="14" spans="2:21" ht="16" thickBot="1">
       <c r="B14" s="71"/>
       <c r="C14" s="121" t="s">
         <v>45</v>
@@ -4995,11 +5030,13 @@
       <c r="P14" s="6"/>
       <c r="Q14" s="18"/>
       <c r="R14" s="6"/>
-      <c r="S14" s="136" t="s">
+      <c r="S14" s="18"/>
+      <c r="T14" s="6"/>
+      <c r="U14" s="136" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="2:19" ht="16" thickBot="1">
+    <row r="15" spans="2:21" ht="16" thickBot="1">
       <c r="B15" s="71"/>
       <c r="C15" s="121" t="s">
         <v>48</v>
@@ -5027,11 +5064,13 @@
       <c r="P15" s="6"/>
       <c r="Q15" s="18"/>
       <c r="R15" s="6"/>
-      <c r="S15" s="136" t="s">
+      <c r="S15" s="18"/>
+      <c r="T15" s="6"/>
+      <c r="U15" s="136" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="2:19" ht="16" thickBot="1">
+    <row r="16" spans="2:21" ht="16" thickBot="1">
       <c r="B16" s="71"/>
       <c r="C16" s="121" t="s">
         <v>47</v>
@@ -5059,11 +5098,13 @@
       <c r="P16" s="6"/>
       <c r="Q16" s="18"/>
       <c r="R16" s="6"/>
-      <c r="S16" s="136" t="s">
+      <c r="S16" s="18"/>
+      <c r="T16" s="6"/>
+      <c r="U16" s="136" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="2:19" ht="16" thickBot="1">
+    <row r="17" spans="2:21" ht="16" thickBot="1">
       <c r="B17" s="71"/>
       <c r="C17" s="121" t="s">
         <v>40</v>
@@ -5091,11 +5132,13 @@
       <c r="P17" s="75"/>
       <c r="Q17" s="18"/>
       <c r="R17" s="75"/>
-      <c r="S17" s="136" t="s">
+      <c r="S17" s="18"/>
+      <c r="T17" s="75"/>
+      <c r="U17" s="136" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="18" spans="2:19" ht="16" thickBot="1">
+    <row r="18" spans="2:21" ht="16" thickBot="1">
       <c r="B18" s="71"/>
       <c r="C18" s="121" t="s">
         <v>46</v>
@@ -5123,7 +5166,9 @@
       <c r="P18" s="75"/>
       <c r="Q18" s="18"/>
       <c r="R18" s="75"/>
-      <c r="S18" s="136" t="s">
+      <c r="S18" s="18"/>
+      <c r="T18" s="75"/>
+      <c r="U18" s="136" t="s">
         <v>88</v>
       </c>
     </row>
@@ -5252,13 +5297,13 @@
         <v>39</v>
       </c>
       <c r="E7" s="187" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="H7" s="48">
         <v>2013</v>
       </c>
       <c r="L7" s="49" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="2:12">
@@ -5269,7 +5314,7 @@
     <row r="9" spans="2:12">
       <c r="B9" s="53"/>
       <c r="C9" s="132" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D9" s="61"/>
       <c r="E9" s="131" t="s">
@@ -5358,7 +5403,7 @@
         <v>2008</v>
       </c>
       <c r="K16" s="49" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="2:11">
@@ -5376,13 +5421,13 @@
         <v>52</v>
       </c>
       <c r="E19" s="48" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H19" s="48">
         <v>2002</v>
       </c>
       <c r="K19" s="49" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="20" spans="2:11">
@@ -5397,13 +5442,13 @@
     <row r="22" spans="2:11">
       <c r="B22" s="53"/>
       <c r="E22" s="48" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H22" s="48">
         <v>2010</v>
       </c>
       <c r="K22" s="49" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="23" spans="2:11">
@@ -5418,7 +5463,7 @@
         <v>2010</v>
       </c>
       <c r="K24" s="49" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="25" spans="2:11">
@@ -5448,8 +5493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y387"/>
   <sheetViews>
-    <sheetView topLeftCell="A380" workbookViewId="0">
-      <selection activeCell="F383" sqref="F383"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6354,10 +6399,10 @@
     <row r="66" spans="2:8" s="139" customFormat="1">
       <c r="B66" s="110"/>
       <c r="D66" s="172" t="s">
+        <v>105</v>
+      </c>
+      <c r="F66" s="140" t="s">
         <v>107</v>
-      </c>
-      <c r="F66" s="140" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="67" spans="2:8" s="139" customFormat="1">
@@ -6423,7 +6468,7 @@
       <c r="B83" s="110"/>
       <c r="D83"/>
       <c r="F83" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H83">
         <v>16.899999999999999</v>
@@ -6432,7 +6477,7 @@
         <v>53</v>
       </c>
       <c r="J83" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="84" spans="2:10" s="139" customFormat="1" ht="16">
@@ -6446,21 +6491,21 @@
         <v>53</v>
       </c>
       <c r="J84" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="85" spans="2:10" s="139" customFormat="1" ht="16">
       <c r="B85" s="110"/>
       <c r="D85"/>
       <c r="F85" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H85" s="179">
         <v>0.12</v>
       </c>
       <c r="I85"/>
       <c r="J85" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="86" spans="2:10" s="139" customFormat="1" ht="16">
@@ -6472,7 +6517,7 @@
       </c>
       <c r="I86"/>
       <c r="J86" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="87" spans="2:10" s="139" customFormat="1">
@@ -6523,7 +6568,7 @@
     <row r="101" spans="2:9" s="139" customFormat="1" ht="16">
       <c r="B101" s="110"/>
       <c r="F101" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H101">
         <v>17.7</v>
@@ -6553,7 +6598,7 @@
     <row r="108" spans="2:9" s="139" customFormat="1">
       <c r="B108" s="110"/>
       <c r="F108" s="140" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H108" s="178">
         <v>0.84</v>
@@ -6574,7 +6619,7 @@
         <v>1216</v>
       </c>
       <c r="F112" s="140" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="113" spans="2:10" s="139" customFormat="1">
@@ -6616,13 +6661,13 @@
     <row r="121" spans="2:10" s="139" customFormat="1">
       <c r="B121" s="110"/>
       <c r="F121" s="180" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H121" s="139">
         <v>22.4</v>
       </c>
       <c r="I121" s="180" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="122" spans="2:10" s="139" customFormat="1">
@@ -6632,7 +6677,7 @@
         <v>22400</v>
       </c>
       <c r="I122" s="180" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="123" spans="2:10" s="139" customFormat="1">
@@ -6642,7 +6687,7 @@
         <v>2240000</v>
       </c>
       <c r="I123" s="180" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="124" spans="2:10" s="139" customFormat="1">
@@ -6657,20 +6702,20 @@
         <v>39648000</v>
       </c>
       <c r="I125" s="180" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="126" spans="2:10" s="139" customFormat="1">
       <c r="B126" s="110"/>
       <c r="F126" s="180" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="H126" s="181">
         <f>H125*H108</f>
         <v>33304320</v>
       </c>
       <c r="I126" s="180" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="127" spans="2:10" s="139" customFormat="1">
@@ -6685,7 +6730,7 @@
         <v>1222</v>
       </c>
       <c r="F129" s="140" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H129" s="172">
         <v>17.7</v>
@@ -6788,7 +6833,7 @@
     <row r="143" spans="1:25" customFormat="1" ht="16">
       <c r="B143" s="110"/>
       <c r="C143" s="182" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D143" s="172"/>
       <c r="E143" s="172"/>
@@ -6820,7 +6865,7 @@
       </c>
       <c r="E144" s="109"/>
       <c r="F144" s="172" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G144" s="172"/>
       <c r="H144" s="172"/>
@@ -6922,7 +6967,7 @@
       <c r="D148" s="172"/>
       <c r="E148" s="109"/>
       <c r="F148" s="173" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G148" s="172"/>
       <c r="H148" s="172"/>
@@ -6976,10 +7021,10 @@
       <c r="F150" s="175"/>
       <c r="G150" s="109"/>
       <c r="H150" s="175" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I150" s="175" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J150" s="175"/>
       <c r="K150" s="172"/>
@@ -7003,7 +7048,7 @@
       <c r="D151" s="175"/>
       <c r="E151" s="109"/>
       <c r="F151" s="175" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G151" s="109"/>
       <c r="H151" s="175">
@@ -7034,7 +7079,7 @@
       <c r="D152" s="175"/>
       <c r="E152" s="109"/>
       <c r="F152" s="175" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G152" s="109"/>
       <c r="H152" s="175">
@@ -7067,10 +7112,10 @@
       <c r="F153" s="175"/>
       <c r="G153" s="109"/>
       <c r="H153" s="175" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="I153" s="175" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="J153" s="175"/>
       <c r="K153" s="172"/>
@@ -7094,7 +7139,7 @@
       <c r="D154" s="175"/>
       <c r="E154" s="109"/>
       <c r="F154" s="175" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G154" s="109"/>
       <c r="H154" s="175">
@@ -7127,7 +7172,7 @@
       <c r="D155" s="175"/>
       <c r="E155" s="109"/>
       <c r="F155" s="175" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G155" s="109"/>
       <c r="H155" s="175">
@@ -7169,7 +7214,7 @@
       </c>
       <c r="J156" s="175"/>
       <c r="K156" s="172" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="L156" s="172"/>
       <c r="M156" s="172"/>
@@ -7191,7 +7236,7 @@
       <c r="D157" s="175"/>
       <c r="E157" s="109"/>
       <c r="F157" s="175" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G157" s="109"/>
       <c r="H157" s="183">
@@ -7227,7 +7272,7 @@
       <c r="D158" s="175"/>
       <c r="E158" s="109"/>
       <c r="F158" s="175" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G158" s="109"/>
       <c r="H158" s="183">
@@ -7291,7 +7336,7 @@
       <c r="D160" s="175"/>
       <c r="E160" s="109"/>
       <c r="F160" s="180" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="G160" s="109"/>
       <c r="H160" s="183">
@@ -7927,7 +7972,7 @@
     <row r="185" spans="1:25" customFormat="1" ht="16">
       <c r="B185" s="110"/>
       <c r="C185" s="172" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D185" s="172"/>
       <c r="E185" s="109"/>
@@ -7957,7 +8002,7 @@
       <c r="D186" s="172"/>
       <c r="E186" s="109"/>
       <c r="F186" s="172" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G186" s="172"/>
       <c r="H186" s="172"/>
@@ -8010,7 +8055,7 @@
       <c r="B188" s="110"/>
       <c r="C188" s="172"/>
       <c r="D188" s="172" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E188" s="109"/>
       <c r="F188" s="172"/>
@@ -8039,10 +8084,13 @@
       <c r="D189" s="172"/>
       <c r="E189" s="109"/>
       <c r="F189" s="184" t="s">
-        <v>108</v>
+        <v>106</v>
+      </c>
+      <c r="G189">
+        <v>17.600000000000001</v>
       </c>
       <c r="H189" s="172" t="s">
-        <v>131</v>
+        <v>165</v>
       </c>
       <c r="I189" s="172"/>
       <c r="J189" s="172"/>
@@ -8068,7 +8116,7 @@
       <c r="E190" s="109"/>
       <c r="F190" s="172"/>
       <c r="H190" s="172" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="I190" s="172"/>
       <c r="J190" s="172"/>
@@ -8097,7 +8145,7 @@
         <v>50</v>
       </c>
       <c r="H191" s="175" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="I191" s="175"/>
       <c r="J191" s="175"/>
@@ -8126,7 +8174,7 @@
         <v>200</v>
       </c>
       <c r="H192" s="175" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="I192" s="175"/>
       <c r="J192" s="175"/>
@@ -8152,10 +8200,10 @@
       <c r="E193" s="109"/>
       <c r="F193" s="175"/>
       <c r="G193" s="175" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="H193" s="175" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I193" s="175"/>
       <c r="J193" s="175"/>
@@ -8181,12 +8229,12 @@
       <c r="E194" s="109"/>
       <c r="F194" s="175"/>
       <c r="G194" s="175" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="H194" s="175"/>
       <c r="I194" s="175"/>
       <c r="J194" s="175" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="K194" s="172"/>
       <c r="L194" s="172"/>
@@ -8209,7 +8257,7 @@
       <c r="D195" s="175"/>
       <c r="E195" s="109"/>
       <c r="F195" s="175" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="G195" s="175">
         <f>50/17500</f>
@@ -8242,7 +8290,7 @@
       <c r="D196" s="175"/>
       <c r="E196" s="109"/>
       <c r="F196" s="175" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G196" s="175">
         <f>200/17500</f>
@@ -8274,7 +8322,7 @@
       <c r="D197" s="175"/>
       <c r="E197" s="175"/>
       <c r="F197" s="175" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="G197" s="175">
         <f>170/17500</f>
@@ -9228,7 +9276,7 @@
       <c r="F235" s="109"/>
       <c r="G235" s="172">
         <f>J258</f>
-        <v>7.7142857142857143E-3</v>
+        <v>7.6704545454545454E-3</v>
       </c>
       <c r="H235" s="175" t="s">
         <v>97</v>
@@ -9260,7 +9308,7 @@
       <c r="F236" s="109"/>
       <c r="G236" s="172">
         <f>N258</f>
-        <v>1.2571428571428572E-2</v>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="H236" s="175" t="s">
         <v>97</v>
@@ -9742,18 +9790,18 @@
       <c r="H255" s="172"/>
       <c r="I255" s="175"/>
       <c r="J255" s="175" t="s">
+        <v>166</v>
+      </c>
+      <c r="K255" s="175" t="s">
         <v>99</v>
-      </c>
-      <c r="K255" s="175" t="s">
-        <v>100</v>
       </c>
       <c r="L255" s="175"/>
       <c r="M255" s="175"/>
       <c r="N255" s="175" t="s">
-        <v>101</v>
+        <v>167</v>
       </c>
       <c r="O255" s="175" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="P255" s="172"/>
       <c r="Q255" s="172"/>
@@ -9778,7 +9826,7 @@
         <v>135</v>
       </c>
       <c r="K256" s="175" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L256" s="175"/>
       <c r="M256" s="175"/>
@@ -9786,7 +9834,7 @@
         <v>220</v>
       </c>
       <c r="O256" s="175" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="P256" s="172"/>
       <c r="Q256" s="172"/>
@@ -9808,20 +9856,20 @@
       <c r="H257" s="172"/>
       <c r="I257" s="175"/>
       <c r="J257" s="175">
-        <f>17.5*1000</f>
-        <v>17500</v>
+        <f>17.6*1000</f>
+        <v>17600</v>
       </c>
       <c r="K257" s="175" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="L257" s="175"/>
       <c r="M257" s="175"/>
       <c r="N257" s="175">
-        <f xml:space="preserve"> 17500</f>
-        <v>17500</v>
+        <f xml:space="preserve"> 17.6 *1000</f>
+        <v>17600</v>
       </c>
       <c r="O257" s="175" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="P257" s="172"/>
       <c r="Q257" s="172"/>
@@ -9844,19 +9892,19 @@
       <c r="I258" s="175"/>
       <c r="J258" s="175">
         <f>J256/J257</f>
-        <v>7.7142857142857143E-3</v>
+        <v>7.6704545454545454E-3</v>
       </c>
       <c r="K258" s="175" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="L258" s="175"/>
       <c r="M258" s="175"/>
       <c r="N258" s="175">
         <f>N256/N257</f>
-        <v>1.2571428571428572E-2</v>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="O258" s="175" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="P258" s="172"/>
       <c r="Q258" s="172"/>
@@ -9928,7 +9976,7 @@
       <c r="H261" s="172"/>
       <c r="I261" s="175"/>
       <c r="J261" s="175" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="K261" s="177">
         <v>0.40100000000000002</v>
@@ -10123,13 +10171,13 @@
     <row r="274" spans="2:10" s="139" customFormat="1">
       <c r="B274" s="110"/>
       <c r="F274" s="180" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H274" s="139">
         <v>10</v>
       </c>
       <c r="I274" s="180" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="275" spans="2:10" s="139" customFormat="1">
@@ -10139,7 +10187,7 @@
         <v>185000</v>
       </c>
       <c r="I275" s="180" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="276" spans="2:10" s="139" customFormat="1">
@@ -10152,7 +10200,7 @@
         <v>56</v>
       </c>
       <c r="J276" s="180" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="277" spans="2:10" s="139" customFormat="1">
@@ -10165,7 +10213,7 @@
         <v>56</v>
       </c>
       <c r="J277" s="180" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="278" spans="2:10" s="139" customFormat="1">
@@ -11039,29 +11087,29 @@
     <row r="380" spans="1:25" ht="16">
       <c r="B380" s="110"/>
       <c r="C380" s="187" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F380" s="189">
         <v>139.09</v>
       </c>
       <c r="G380" s="172" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="H380" s="190" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="I380" s="191">
         <v>41327</v>
       </c>
       <c r="J380" s="192" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="381" spans="1:25">
       <c r="B381" s="110"/>
       <c r="F381" s="205">
         <f>'Research data'!G8</f>
-        <v>18.100000000000001</v>
+        <v>18</v>
       </c>
       <c r="G381" s="172" t="s">
         <v>53</v>
@@ -11072,17 +11120,17 @@
       <c r="B382" s="110"/>
       <c r="F382" s="109">
         <f>F381*1000</f>
-        <v>18100</v>
+        <v>18000</v>
       </c>
       <c r="G382" s="204" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="383" spans="1:25">
       <c r="B383" s="110"/>
       <c r="F383" s="206">
         <f>F380/F382</f>
-        <v>7.6845303867403318E-3</v>
+        <v>7.7272222222222221E-3</v>
       </c>
     </row>
     <row r="384" spans="1:25">

</xml_diff>